<commit_message>
Implement login for anseco demo
</commit_message>
<xml_diff>
--- a/sheet_engine/static/template_sheets/class_teacher_remarks.xlsx
+++ b/sheet_engine/static/template_sheets/class_teacher_remarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeLab\Projects\curie\sheet_engine\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrd/Documents/repositories/curie/sheet_engine/static/template_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17539C8-FFCB-495F-A5C2-720B7AC71302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8F96C3-4AB2-0345-9EB7-4F8D3568FB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{751BF1E8-C5A7-4578-BDEB-D67A1084152A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19920" xr2:uid="{751BF1E8-C5A7-4578-BDEB-D67A1084152A}"/>
   </bookViews>
   <sheets>
     <sheet name="class_teacher_remarks" sheetId="1" r:id="rId1"/>
@@ -135,22 +135,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>123039</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>189546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FC854E1-C077-4D1C-A9BE-B4B3F1FEEC89}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6DF2347-16B9-624F-9F09-710FEE9C38AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -159,71 +159,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3143250" y="57150"/>
-          <a:ext cx="1332714" cy="1438275"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123039</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D51BF29E-0409-4E0C-91CC-8E328C817627}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4486275" y="57150"/>
-          <a:ext cx="1332714" cy="1438275"/>
+          <a:off x="3263900" y="203200"/>
+          <a:ext cx="1231900" cy="1319846"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -538,18 +482,18 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -560,7 +504,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -571,7 +515,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -582,7 +526,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -593,7 +537,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -604,7 +548,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -615,7 +559,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -626,7 +570,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -637,7 +581,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -648,7 +592,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -659,7 +603,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>

</xml_diff>